<commit_message>
added from batch file
</commit_message>
<xml_diff>
--- a/NOMAC_Work Order Manangement.xlsx
+++ b/NOMAC_Work Order Manangement.xlsx
@@ -28887,7 +28887,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K510"/>
+  <dimension ref="A1:K410"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
@@ -29156,7 +29156,7 @@
       </c>
       <c r="E12" s="16" t="inlineStr">
         <is>
-          <t>Enter lname3 in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F12" s="38" t="inlineStr">
@@ -29186,7 +29186,7 @@
       </c>
       <c r="E14" s="16" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F14" s="38" t="inlineStr">
@@ -29221,7 +29221,7 @@
       </c>
       <c r="E16" s="16" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F16" s="35" t="inlineStr">
@@ -29236,7 +29236,7 @@
       </c>
       <c r="E17" s="16" t="inlineStr">
         <is>
-          <t>Enter hello in comment Field</t>
+          <t>Enter 111 in comment Field</t>
         </is>
       </c>
       <c r="F17" s="35" t="inlineStr">
@@ -29251,7 +29251,7 @@
       </c>
       <c r="E18" s="16" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F18" s="35" t="inlineStr">
@@ -29319,7 +29319,7 @@
       </c>
       <c r="E22" s="16" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F22" s="38" t="inlineStr">
@@ -29389,7 +29389,7 @@
       </c>
       <c r="E26" s="16" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload nan in file2upload Field</t>
         </is>
       </c>
       <c r="F26" s="41" t="inlineStr">
@@ -29459,7 +29459,7 @@
       </c>
       <c r="E30" s="36" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F30" s="35" t="inlineStr">
@@ -29479,7 +29479,7 @@
       </c>
       <c r="E31" s="36" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F31" s="35" t="inlineStr">
@@ -29494,7 +29494,7 @@
       </c>
       <c r="E32" s="36" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F32" s="35" t="inlineStr">
@@ -29524,7 +29524,7 @@
       </c>
       <c r="E34" s="36" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload nan in file2upload Field</t>
         </is>
       </c>
       <c r="F34" s="35" t="inlineStr">
@@ -29559,7 +29559,7 @@
       </c>
       <c r="E36" s="36" t="inlineStr">
         <is>
-          <t>Enter lname3 in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F36" s="35" t="inlineStr">
@@ -29589,7 +29589,7 @@
       </c>
       <c r="E38" s="36" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F38" s="35" t="inlineStr">
@@ -29609,7 +29609,7 @@
       </c>
       <c r="E39" s="36" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F39" s="35" t="inlineStr">
@@ -29624,7 +29624,7 @@
       </c>
       <c r="E40" s="36" t="inlineStr">
         <is>
-          <t>Enter lname3 in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F40" s="35" t="inlineStr">
@@ -29654,7 +29654,7 @@
       </c>
       <c r="E42" s="36" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F42" s="35" t="inlineStr">
@@ -29689,7 +29689,7 @@
       </c>
       <c r="E44" s="36" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter lname3 in Lname Field</t>
         </is>
       </c>
       <c r="F44" s="35" t="inlineStr">
@@ -29704,7 +29704,7 @@
       </c>
       <c r="E45" s="36" t="inlineStr">
         <is>
-          <t>Enter 111 in comment Field</t>
+          <t>Enter hello in comment Field</t>
         </is>
       </c>
       <c r="F45" s="35" t="inlineStr">
@@ -29719,7 +29719,7 @@
       </c>
       <c r="E46" s="36" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F46" s="35" t="inlineStr">
@@ -29769,7 +29769,7 @@
       </c>
       <c r="E49" s="37" t="inlineStr">
         <is>
-          <t>Enter 111 in comment Field</t>
+          <t>Enter hello in comment Field</t>
         </is>
       </c>
       <c r="F49" s="22" t="inlineStr">
@@ -29784,7 +29784,7 @@
       </c>
       <c r="E50" s="20" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F50" s="35" t="inlineStr">
@@ -29804,7 +29804,7 @@
       </c>
       <c r="E51" s="20" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F51" s="35" t="inlineStr">
@@ -29834,7 +29834,7 @@
       </c>
       <c r="E53" s="20" t="inlineStr">
         <is>
-          <t>Enter 111 in comment Field</t>
+          <t>Enter hello in comment Field</t>
         </is>
       </c>
       <c r="F53" s="35" t="inlineStr">
@@ -29849,7 +29849,7 @@
       </c>
       <c r="E54" s="20" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F54" s="35" t="inlineStr">
@@ -29869,7 +29869,7 @@
       </c>
       <c r="E55" s="20" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F55" s="35" t="inlineStr">
@@ -29886,7 +29886,7 @@
       </c>
       <c r="E56" s="20" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F56" s="35" t="inlineStr">
@@ -29920,7 +29920,7 @@
       </c>
       <c r="E58" s="20" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F58" s="35" t="inlineStr">
@@ -29958,7 +29958,7 @@
       </c>
       <c r="E60" s="20" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter lname3 in Lname Field</t>
         </is>
       </c>
       <c r="F60" s="35" t="inlineStr">
@@ -29992,7 +29992,7 @@
       </c>
       <c r="E62" s="20" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F62" s="35" t="inlineStr">
@@ -30030,7 +30030,7 @@
       </c>
       <c r="E64" s="20" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter lname3 in Lname Field</t>
         </is>
       </c>
       <c r="F64" s="35" t="inlineStr">
@@ -30047,7 +30047,7 @@
       </c>
       <c r="E65" s="20" t="inlineStr">
         <is>
-          <t>Enter hello in comment Field</t>
+          <t>Enter 111 in comment Field</t>
         </is>
       </c>
       <c r="F65" s="35" t="inlineStr">
@@ -30064,7 +30064,7 @@
       </c>
       <c r="E66" s="20" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F66" s="35" t="inlineStr">
@@ -30085,7 +30085,7 @@
       </c>
       <c r="E67" s="20" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F67" s="35" t="inlineStr">
@@ -30102,7 +30102,7 @@
       </c>
       <c r="E68" s="20" t="inlineStr">
         <is>
-          <t>Enter lname3 in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F68" s="35" t="inlineStr">
@@ -30119,7 +30119,7 @@
       </c>
       <c r="E69" s="20" t="inlineStr">
         <is>
-          <t>Enter 111 in comment Field</t>
+          <t>Enter hello in comment Field</t>
         </is>
       </c>
       <c r="F69" s="35" t="inlineStr">
@@ -30136,7 +30136,7 @@
       </c>
       <c r="E70" s="20" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F70" s="35" t="inlineStr">
@@ -30157,7 +30157,7 @@
       </c>
       <c r="E71" s="20" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F71" s="20" t="inlineStr">
@@ -30174,7 +30174,7 @@
       </c>
       <c r="E72" s="20" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter lname3 in Lname Field</t>
         </is>
       </c>
       <c r="F72" s="20" t="inlineStr">
@@ -30208,7 +30208,7 @@
       </c>
       <c r="E74" s="20" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F74" s="20" t="inlineStr">
@@ -30229,7 +30229,7 @@
       </c>
       <c r="E75" s="20" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F75" s="20" t="inlineStr">
@@ -30280,7 +30280,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F78" s="13" t="inlineStr">
@@ -30330,7 +30330,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Enter hello in comment Field</t>
+          <t>Enter 111 in comment Field</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -30345,7 +30345,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -30365,7 +30365,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -30410,7 +30410,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -30445,7 +30445,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -30460,7 +30460,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Enter hello in comment Field</t>
+          <t>Enter 111 in comment Field</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -30475,7 +30475,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -30495,7 +30495,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -30540,7 +30540,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -30560,7 +30560,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -30575,7 +30575,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter lname3 in Lname Field</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -30605,7 +30605,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload nan in file2upload Field</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -30655,7 +30655,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Enter 111 in comment Field</t>
+          <t>Enter hello in comment Field</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -30670,7 +30670,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -30735,7 +30735,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -30770,7 +30770,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Enter lname3 in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -30800,7 +30800,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -30865,7 +30865,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -30930,7 +30930,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -30965,7 +30965,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -30980,7 +30980,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Enter hello in comment Field</t>
+          <t>Enter 111 in comment Field</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -30995,7 +30995,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -31015,7 +31015,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -31030,7 +31030,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -31060,7 +31060,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -31080,7 +31080,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -31095,7 +31095,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter lname3 in Lname Field</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -31125,7 +31125,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -31145,7 +31145,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -31160,7 +31160,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -31190,7 +31190,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -31210,7 +31210,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -31255,7 +31255,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -31290,7 +31290,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter lname3 in Lname Field</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -31320,7 +31320,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload nan in file2upload Field</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -31355,7 +31355,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Enter lname3 in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -31385,7 +31385,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -31450,7 +31450,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -31470,7 +31470,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -31485,7 +31485,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>Enter lname3 in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -31515,7 +31515,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -31535,7 +31535,7 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -31580,7 +31580,7 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -31600,7 +31600,7 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -31615,7 +31615,7 @@
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -31645,7 +31645,7 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -31680,7 +31680,7 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter lname3 in Lname Field</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -31710,7 +31710,7 @@
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -31745,7 +31745,7 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>Enter lname3 in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -31775,7 +31775,7 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -31840,7 +31840,7 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -31860,7 +31860,7 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -31875,7 +31875,7 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -31890,7 +31890,7 @@
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>Enter hello in comment Field</t>
+          <t>Enter 111 in comment Field</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -31905,7 +31905,7 @@
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -31940,7 +31940,7 @@
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
@@ -31970,7 +31970,7 @@
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -31990,7 +31990,7 @@
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -32005,7 +32005,7 @@
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
@@ -32035,7 +32035,7 @@
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -32070,7 +32070,7 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -32085,7 +32085,7 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>Enter 111 in comment Field</t>
+          <t>Enter hello in comment Field</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
@@ -32100,7 +32100,7 @@
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -32165,7 +32165,7 @@
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -32200,7 +32200,7 @@
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -32230,7 +32230,7 @@
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -32250,7 +32250,7 @@
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
@@ -32265,7 +32265,7 @@
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
@@ -32280,7 +32280,7 @@
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>Enter 111 in comment Field</t>
+          <t>Enter hello in comment Field</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -32295,7 +32295,7 @@
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -32360,7 +32360,7 @@
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -32395,7 +32395,7 @@
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>Enter lname3 in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -32410,7 +32410,7 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>Enter 111 in comment Field</t>
+          <t>Enter hello in comment Field</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -32425,7 +32425,7 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload nan in file2upload Field</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -32445,7 +32445,7 @@
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -32460,7 +32460,7 @@
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>Enter lname3 in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -32490,7 +32490,7 @@
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload nan in file2upload Field</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -32510,7 +32510,7 @@
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -32525,7 +32525,7 @@
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -32555,7 +32555,7 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload nan in file2upload Field</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -32590,7 +32590,7 @@
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter lname3 in Lname Field</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -32620,7 +32620,7 @@
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload nan in file2upload Field</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -32655,7 +32655,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -32685,7 +32685,7 @@
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload nan in file2upload Field</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -32705,7 +32705,7 @@
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -32720,7 +32720,7 @@
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -32750,7 +32750,7 @@
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -32785,7 +32785,7 @@
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -32815,7 +32815,7 @@
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -32850,7 +32850,7 @@
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -32880,7 +32880,7 @@
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
@@ -32915,7 +32915,7 @@
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -32930,7 +32930,7 @@
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>Enter hello in comment Field</t>
+          <t>Enter 111 in comment Field</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -32995,7 +32995,7 @@
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>Enter hello in comment Field</t>
+          <t>Enter 111 in comment Field</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
@@ -33010,7 +33010,7 @@
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
@@ -33030,7 +33030,7 @@
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F247" t="inlineStr">
@@ -33045,7 +33045,7 @@
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>Enter lname3 in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F248" t="inlineStr">
@@ -33075,7 +33075,7 @@
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload nan in file2upload Field</t>
         </is>
       </c>
       <c r="F250" t="inlineStr">
@@ -33110,7 +33110,7 @@
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter lname3 in Lname Field</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
@@ -33140,7 +33140,7 @@
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F254" t="inlineStr">
@@ -33175,7 +33175,7 @@
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter lname3 in Lname Field</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
@@ -33205,7 +33205,7 @@
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F258" t="inlineStr">
@@ -33240,7 +33240,7 @@
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter lname3 in Lname Field</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -33270,7 +33270,7 @@
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
@@ -33305,7 +33305,7 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
@@ -33335,7 +33335,7 @@
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -33355,7 +33355,7 @@
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
@@ -33400,7 +33400,7 @@
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
@@ -33420,7 +33420,7 @@
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -33435,7 +33435,7 @@
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter lname3 in Lname Field</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
@@ -33450,7 +33450,7 @@
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>Enter hello in comment Field</t>
+          <t>Enter 111 in comment Field</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
@@ -33465,7 +33465,7 @@
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
@@ -33500,7 +33500,7 @@
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>Enter lname3 in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -33515,7 +33515,7 @@
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>Enter 111 in comment Field</t>
+          <t>Enter hello in comment Field</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -33530,7 +33530,7 @@
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
@@ -33550,7 +33550,7 @@
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
@@ -33565,7 +33565,7 @@
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
@@ -33595,7 +33595,7 @@
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -33645,7 +33645,7 @@
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>Enter 111 in comment Field</t>
+          <t>Enter hello in comment Field</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -33660,7 +33660,7 @@
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -33680,7 +33680,7 @@
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -33725,7 +33725,7 @@
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
@@ -33760,7 +33760,7 @@
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -33790,7 +33790,7 @@
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -33810,7 +33810,7 @@
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
@@ -33840,7 +33840,7 @@
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>Enter hello in comment Field</t>
+          <t>Enter 111 in comment Field</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
@@ -33855,7 +33855,7 @@
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
@@ -33890,7 +33890,7 @@
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>Enter lname3 in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
@@ -33905,7 +33905,7 @@
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>Enter hello in comment Field</t>
+          <t>Enter 111 in comment Field</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
@@ -33920,7 +33920,7 @@
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
@@ -33955,7 +33955,7 @@
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
@@ -34005,7 +34005,7 @@
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
@@ -34035,7 +34035,7 @@
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>Enter hello in comment Field</t>
+          <t>Enter 111 in comment Field</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -34050,7 +34050,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
@@ -34085,7 +34085,7 @@
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
@@ -34100,7 +34100,7 @@
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>Enter 111 in comment Field</t>
+          <t>Enter hello in comment Field</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -34115,7 +34115,7 @@
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
@@ -34150,7 +34150,7 @@
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>Enter lname3 in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
@@ -34165,7 +34165,7 @@
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>Enter hello in comment Field</t>
+          <t>Enter 111 in comment Field</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
@@ -34180,7 +34180,7 @@
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
@@ -34200,7 +34200,7 @@
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
@@ -34215,7 +34215,7 @@
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
@@ -34245,7 +34245,7 @@
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
@@ -34280,7 +34280,7 @@
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
@@ -34310,7 +34310,7 @@
       </c>
       <c r="E326" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
@@ -34330,7 +34330,7 @@
       </c>
       <c r="E327" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
@@ -34345,7 +34345,7 @@
       </c>
       <c r="E328" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F328" t="inlineStr">
@@ -34375,7 +34375,7 @@
       </c>
       <c r="E330" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F330" t="inlineStr">
@@ -34395,7 +34395,7 @@
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F331" t="inlineStr">
@@ -34410,7 +34410,7 @@
       </c>
       <c r="E332" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F332" t="inlineStr">
@@ -34440,7 +34440,7 @@
       </c>
       <c r="E334" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F334" t="inlineStr">
@@ -34475,7 +34475,7 @@
       </c>
       <c r="E336" t="inlineStr">
         <is>
-          <t>Enter lname3 in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F336" t="inlineStr">
@@ -34505,7 +34505,7 @@
       </c>
       <c r="E338" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F338" t="inlineStr">
@@ -34540,7 +34540,7 @@
       </c>
       <c r="E340" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F340" t="inlineStr">
@@ -34570,7 +34570,7 @@
       </c>
       <c r="E342" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload nan in file2upload Field</t>
         </is>
       </c>
       <c r="F342" t="inlineStr">
@@ -34590,7 +34590,7 @@
       </c>
       <c r="E343" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F343" t="inlineStr">
@@ -34635,7 +34635,7 @@
       </c>
       <c r="E346" t="inlineStr">
         <is>
-          <t>Upload nan in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F346" t="inlineStr">
@@ -34655,7 +34655,7 @@
       </c>
       <c r="E347" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F347" t="inlineStr">
@@ -34670,7 +34670,7 @@
       </c>
       <c r="E348" t="inlineStr">
         <is>
-          <t>Enter lname3 in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F348" t="inlineStr">
@@ -34700,7 +34700,7 @@
       </c>
       <c r="E350" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F350" t="inlineStr">
@@ -34720,7 +34720,7 @@
       </c>
       <c r="E351" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F351" t="inlineStr">
@@ -34735,7 +34735,7 @@
       </c>
       <c r="E352" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F352" t="inlineStr">
@@ -34750,7 +34750,7 @@
       </c>
       <c r="E353" t="inlineStr">
         <is>
-          <t>Enter 111 in comment Field</t>
+          <t>Enter hello in comment Field</t>
         </is>
       </c>
       <c r="F353" t="inlineStr">
@@ -34765,7 +34765,7 @@
       </c>
       <c r="E354" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F354" t="inlineStr">
@@ -34785,7 +34785,7 @@
       </c>
       <c r="E355" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F355" t="inlineStr">
@@ -34830,7 +34830,7 @@
       </c>
       <c r="E358" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F358" t="inlineStr">
@@ -34865,7 +34865,7 @@
       </c>
       <c r="E360" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F360" t="inlineStr">
@@ -34880,7 +34880,7 @@
       </c>
       <c r="E361" t="inlineStr">
         <is>
-          <t>Enter hello in comment Field</t>
+          <t>Enter 111 in comment Field</t>
         </is>
       </c>
       <c r="F361" t="inlineStr">
@@ -34895,7 +34895,7 @@
       </c>
       <c r="E362" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F362" t="inlineStr">
@@ -34915,7 +34915,7 @@
       </c>
       <c r="E363" t="inlineStr">
         <is>
-          <t>Enter John in first Field</t>
+          <t>Enter Johnny in first Field</t>
         </is>
       </c>
       <c r="F363" t="inlineStr">
@@ -34930,7 +34930,7 @@
       </c>
       <c r="E364" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F364" t="inlineStr">
@@ -34945,7 +34945,7 @@
       </c>
       <c r="E365" t="inlineStr">
         <is>
-          <t>Enter hello in comment Field</t>
+          <t>Enter 111 in comment Field</t>
         </is>
       </c>
       <c r="F365" t="inlineStr">
@@ -34960,7 +34960,7 @@
       </c>
       <c r="E366" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F366" t="inlineStr">
@@ -34995,7 +34995,7 @@
       </c>
       <c r="E368" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F368" t="inlineStr">
@@ -35090,7 +35090,7 @@
       </c>
       <c r="E374" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F374" t="inlineStr">
@@ -35110,7 +35110,7 @@
       </c>
       <c r="E375" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F375" t="inlineStr">
@@ -35155,7 +35155,7 @@
       </c>
       <c r="E378" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F378" t="inlineStr">
@@ -35190,7 +35190,7 @@
       </c>
       <c r="E380" t="inlineStr">
         <is>
-          <t>Enter lname3 in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F380" t="inlineStr">
@@ -35220,7 +35220,7 @@
       </c>
       <c r="E382" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload nan in file2upload Field</t>
         </is>
       </c>
       <c r="F382" t="inlineStr">
@@ -35255,7 +35255,7 @@
       </c>
       <c r="E384" t="inlineStr">
         <is>
-          <t>Enter Smith in Lname Field</t>
+          <t>Enter New in Lname Field</t>
         </is>
       </c>
       <c r="F384" t="inlineStr">
@@ -35285,7 +35285,7 @@
       </c>
       <c r="E386" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F386" t="inlineStr">
@@ -35320,7 +35320,7 @@
       </c>
       <c r="E388" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F388" t="inlineStr">
@@ -35350,7 +35350,7 @@
       </c>
       <c r="E390" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F390" t="inlineStr">
@@ -35370,7 +35370,7 @@
       </c>
       <c r="E391" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F391" t="inlineStr">
@@ -35415,7 +35415,7 @@
       </c>
       <c r="E394" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F394" t="inlineStr">
@@ -35435,7 +35435,7 @@
       </c>
       <c r="E395" t="inlineStr">
         <is>
-          <t>Enter Johnny in first Field</t>
+          <t>Enter John in first Field</t>
         </is>
       </c>
       <c r="F395" t="inlineStr">
@@ -35465,7 +35465,7 @@
       </c>
       <c r="E397" t="inlineStr">
         <is>
-          <t>Enter 111 in comment Field</t>
+          <t>Enter hello in comment Field</t>
         </is>
       </c>
       <c r="F397" t="inlineStr">
@@ -35480,7 +35480,7 @@
       </c>
       <c r="E398" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F398" t="inlineStr">
@@ -35515,7 +35515,7 @@
       </c>
       <c r="E400" t="inlineStr">
         <is>
-          <t>Enter New in Lname Field</t>
+          <t>Enter Smith in Lname Field</t>
         </is>
       </c>
       <c r="F400" t="inlineStr">
@@ -35545,7 +35545,7 @@
       </c>
       <c r="E402" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F402" t="inlineStr">
@@ -35595,7 +35595,7 @@
       </c>
       <c r="E405" t="inlineStr">
         <is>
-          <t>Enter hello in comment Field</t>
+          <t>Enter 111 in comment Field</t>
         </is>
       </c>
       <c r="F405" t="inlineStr">
@@ -35610,7 +35610,7 @@
       </c>
       <c r="E406" t="inlineStr">
         <is>
-          <t>Upload C:\users\johnny\file3.pdf in file2upload Field</t>
+          <t>Upload C:\Users\johnny.abouhaidar\Desktop\myfiles\katalon\Test Run Report 26.pdf in file2upload Field</t>
         </is>
       </c>
       <c r="F406" t="inlineStr">
@@ -35684,106 +35684,6 @@
         </is>
       </c>
     </row>
-    <row r="411"/>
-    <row r="412"/>
-    <row r="413"/>
-    <row r="414"/>
-    <row r="415"/>
-    <row r="416"/>
-    <row r="417"/>
-    <row r="418"/>
-    <row r="419"/>
-    <row r="420"/>
-    <row r="421"/>
-    <row r="422"/>
-    <row r="423"/>
-    <row r="424"/>
-    <row r="425"/>
-    <row r="426"/>
-    <row r="427"/>
-    <row r="428"/>
-    <row r="429"/>
-    <row r="430"/>
-    <row r="431"/>
-    <row r="432"/>
-    <row r="433"/>
-    <row r="434"/>
-    <row r="435"/>
-    <row r="436"/>
-    <row r="437"/>
-    <row r="438"/>
-    <row r="439"/>
-    <row r="440"/>
-    <row r="441"/>
-    <row r="442"/>
-    <row r="443"/>
-    <row r="444"/>
-    <row r="445"/>
-    <row r="446"/>
-    <row r="447"/>
-    <row r="448"/>
-    <row r="449"/>
-    <row r="450"/>
-    <row r="451"/>
-    <row r="452"/>
-    <row r="453"/>
-    <row r="454"/>
-    <row r="455"/>
-    <row r="456"/>
-    <row r="457"/>
-    <row r="458"/>
-    <row r="459"/>
-    <row r="460"/>
-    <row r="461"/>
-    <row r="462"/>
-    <row r="463"/>
-    <row r="464"/>
-    <row r="465"/>
-    <row r="466"/>
-    <row r="467"/>
-    <row r="468"/>
-    <row r="469"/>
-    <row r="470"/>
-    <row r="471"/>
-    <row r="472"/>
-    <row r="473"/>
-    <row r="474"/>
-    <row r="475"/>
-    <row r="476"/>
-    <row r="477"/>
-    <row r="478"/>
-    <row r="479"/>
-    <row r="480"/>
-    <row r="481"/>
-    <row r="482"/>
-    <row r="483"/>
-    <row r="484"/>
-    <row r="485"/>
-    <row r="486"/>
-    <row r="487"/>
-    <row r="488"/>
-    <row r="489"/>
-    <row r="490"/>
-    <row r="491"/>
-    <row r="492"/>
-    <row r="493"/>
-    <row r="494"/>
-    <row r="495"/>
-    <row r="496"/>
-    <row r="497"/>
-    <row r="498"/>
-    <row r="499"/>
-    <row r="500"/>
-    <row r="501"/>
-    <row r="502"/>
-    <row r="503"/>
-    <row r="504"/>
-    <row r="505"/>
-    <row r="506"/>
-    <row r="507"/>
-    <row r="508"/>
-    <row r="509"/>
-    <row r="510"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="K22:K28"/>

</xml_diff>